<commit_message>
BR3 and start of BR4
</commit_message>
<xml_diff>
--- a/CA1/TestPlan-Beampro.xlsx
+++ b/CA1/TestPlan-Beampro.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="37460" windowHeight="21160" activeTab="2"/>
+    <workbookView xWindow="-28800" yWindow="3600" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
     <sheet name="Business Requirement 1 General" sheetId="4" r:id="rId2"/>
     <sheet name="Requirement 2 Sign Up" sheetId="5" r:id="rId3"/>
     <sheet name="Requirement 3 Login" sheetId="7" r:id="rId4"/>
-    <sheet name="Test Progress" sheetId="6" r:id="rId5"/>
+    <sheet name="Requirement 4 Forum" sheetId="9" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
+    <sheet name="Test Progress" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="162">
   <si>
     <t>Project Name</t>
   </si>
@@ -525,6 +527,82 @@
   </si>
   <si>
     <t>Total Test Cases: 9</t>
+  </si>
+  <si>
+    <t>Password Reset</t>
+  </si>
+  <si>
+    <t>There will be an option to reset a password if forgotten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensures the user receives an email with options to reset the password
+</t>
+  </si>
+  <si>
+    <t>User receives an email if a matching email is provided</t>
+  </si>
+  <si>
+    <t>Return to Beam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upon loading the forums there should be an option to bring user 
+'back to beam'
+</t>
+  </si>
+  <si>
+    <t>User can navagate back to beam easily</t>
+  </si>
+  <si>
+    <t>Button with the text 'Back to Beam' is there.</t>
+  </si>
+  <si>
+    <t>TC4.1</t>
+  </si>
+  <si>
+    <t>Recent posts</t>
+  </si>
+  <si>
+    <t>Navagate to Forums page 
+A button should be present to bring up recent posts across all catagories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Users can view recent posts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button provides a view with recent posts. </t>
+  </si>
+  <si>
+    <t>TC4.2</t>
+  </si>
+  <si>
+    <t>TC4.3</t>
+  </si>
+  <si>
+    <t>Catagories View</t>
+  </si>
+  <si>
+    <t>Navagate to Forums page 
+A button should be present to bring the user to a catagories view with parent catagories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button brings the user a view of catagories.
+Users can view recent posts </t>
+  </si>
+  <si>
+    <t>Button works a expected</t>
+  </si>
+  <si>
+    <t>Ryan Gordon</t>
+  </si>
+  <si>
+    <t>Completed BR 1+2</t>
+  </si>
+  <si>
+    <t>Completed BR 3</t>
+  </si>
+  <si>
+    <t>Completed BR 4</t>
   </si>
 </sst>
 </file>
@@ -1203,9 +1281,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1334,78 +1409,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
@@ -1432,11 +1435,294 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="75">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2051,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2076,9 +2362,9 @@
     <row r="2" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="84"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2108,11 +2394,11 @@
     <row r="6" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="75"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -2121,10 +2407,10 @@
       <c r="C7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="77"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -2133,10 +2419,10 @@
       <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="79"/>
+      <c r="E8" s="91"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2161,10 +2447,10 @@
       <c r="C11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="80" t="s">
+      <c r="D11" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="81"/>
+      <c r="E11" s="93"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2173,10 +2459,10 @@
       <c r="C12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="82" t="s">
+      <c r="D12" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="83"/>
+      <c r="E12" s="95"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2185,8 +2471,8 @@
       <c r="C13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="78"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2224,11 +2510,11 @@
     <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="68"/>
-      <c r="E18" s="69"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2268,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>33</v>
+        <v>158</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>9</v>
@@ -2278,201 +2564,219 @@
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="12"/>
+      <c r="C23" s="17">
+        <v>2</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>159</v>
+      </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="23"/>
+      <c r="C24" s="17">
+        <v>3</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>160</v>
+      </c>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23"/>
+      <c r="C25" s="17">
+        <v>4</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>161</v>
+      </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="6"/>
       <c r="C26" s="20"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="6"/>
       <c r="C27" s="20"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="6"/>
       <c r="C28" s="20"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="6"/>
       <c r="C29" s="20"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="24"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="6"/>
       <c r="C30" s="20"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="23"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="6"/>
       <c r="C31" s="20"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="23"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="6"/>
       <c r="C32" s="20"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="24"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="6"/>
       <c r="C33" s="20"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="24"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="6"/>
       <c r="C34" s="20"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="24"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="6"/>
       <c r="C35" s="20"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="24"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="23"/>
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="6"/>
       <c r="C36" s="20"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="24"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="6"/>
       <c r="C37" s="20"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="24"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="6"/>
       <c r="C38" s="20"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="24"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="6"/>
       <c r="C39" s="20"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="24"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="23"/>
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="6"/>
       <c r="C40" s="20"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="24"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="23"/>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="6"/>
       <c r="C41" s="20"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="24"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="6"/>
       <c r="C42" s="20"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="24"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="6"/>
       <c r="C43" s="20"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="24"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="23"/>
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="6"/>
       <c r="C44" s="20"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="24"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="6"/>
       <c r="C45" s="20"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="24"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="23"/>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="6"/>
       <c r="C46" s="20"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="24"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="27"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="26"/>
       <c r="F47" s="4"/>
     </row>
   </sheetData>
@@ -2515,553 +2819,553 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62" t="s">
+      <c r="A1" s="60"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="97" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="85" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="54" t="s">
+      <c r="L3" s="53" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="60" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="59">
+    <row r="4" spans="1:12" s="59" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="56">
         <v>1</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="J4" s="57" t="s">
+      <c r="J4" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-    </row>
-    <row r="5" spans="1:12" s="60" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="59">
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+    </row>
+    <row r="5" spans="1:12" s="59" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="58">
         <v>1.2</v>
       </c>
-      <c r="B5" s="57">
+      <c r="B5" s="56">
         <v>1</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="I5" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="57" t="s">
+      <c r="J5" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="58"/>
-      <c r="L5" s="57"/>
-    </row>
-    <row r="6" spans="1:12" s="60" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A6" s="59">
+      <c r="K5" s="57"/>
+      <c r="L5" s="56"/>
+    </row>
+    <row r="6" spans="1:12" s="59" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A6" s="58">
         <v>1.3</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="56">
         <v>1</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="I6" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="57" t="s">
+      <c r="J6" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-    </row>
-    <row r="7" spans="1:12" s="60" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A7" s="59">
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+    </row>
+    <row r="7" spans="1:12" s="59" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A7" s="58">
         <v>1.4</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B7" s="56">
         <v>1</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="56" t="s">
+      <c r="G7" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="57" t="s">
+      <c r="I7" s="55"/>
+      <c r="J7" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="58" t="s">
+      <c r="K7" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="L7" s="57"/>
-    </row>
-    <row r="8" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57"/>
-    </row>
-    <row r="9" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="59"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-    </row>
-    <row r="10" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="59"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-    </row>
-    <row r="11" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-    </row>
-    <row r="12" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="59"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-    </row>
-    <row r="13" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-    </row>
-    <row r="14" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-    </row>
-    <row r="15" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-    </row>
-    <row r="16" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-    </row>
-    <row r="17" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="57"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-    </row>
-    <row r="18" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="57"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-    </row>
-    <row r="19" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-    </row>
-    <row r="20" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="57"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-    </row>
-    <row r="21" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="57"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-    </row>
-    <row r="22" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="57"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-    </row>
-    <row r="23" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-    </row>
-    <row r="24" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="57"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-    </row>
-    <row r="25" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="57"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-    </row>
-    <row r="26" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-    </row>
-    <row r="27" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="57"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-    </row>
-    <row r="28" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="57"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-    </row>
-    <row r="29" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="57"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
-    </row>
-    <row r="30" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="57"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-    </row>
-    <row r="31" spans="1:12" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="57"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
+      <c r="L7" s="56"/>
+    </row>
+    <row r="8" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="58"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+    </row>
+    <row r="9" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="58"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+    </row>
+    <row r="10" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="58"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+    </row>
+    <row r="11" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="58"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+    </row>
+    <row r="12" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="58"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+    </row>
+    <row r="13" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="58"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+    </row>
+    <row r="14" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="56"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+    </row>
+    <row r="15" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="56"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+    </row>
+    <row r="16" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="56"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+    </row>
+    <row r="17" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+    </row>
+    <row r="18" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+    </row>
+    <row r="19" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="56"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="56"/>
+    </row>
+    <row r="20" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="56"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+    </row>
+    <row r="21" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="56"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+    </row>
+    <row r="22" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="56"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+    </row>
+    <row r="23" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="56"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+    </row>
+    <row r="24" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="56"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+    </row>
+    <row r="25" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="56"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+    </row>
+    <row r="26" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="56"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+    </row>
+    <row r="27" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="56"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+    </row>
+    <row r="28" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="56"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+    </row>
+    <row r="29" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="56"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+    </row>
+    <row r="30" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="56"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+    </row>
+    <row r="31" spans="1:12" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="56"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F32" s="63"/>
+      <c r="F32" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3070,13 +3374,13 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="44" priority="1" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="74" priority="1" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="73" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="3" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="72" priority="3" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3088,7 +3392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -3107,307 +3411,307 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="33" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-    </row>
-    <row r="3" spans="1:10" s="52" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" s="51" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="A4" s="94">
+      <c r="A4" s="69">
         <v>2.1</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="97" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="99" t="s">
+      <c r="E4" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="57" t="s">
+      <c r="I4" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="94">
+      <c r="A5" s="69">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="97" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="90" t="s">
+      <c r="D5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="98" t="s">
+      <c r="E5" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="91" t="s">
+      <c r="F5" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="91" t="s">
+      <c r="G5" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="91" t="s">
+      <c r="H5" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.2">
-      <c r="A6" s="94">
+      <c r="A6" s="69">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="97" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="98" t="s">
+      <c r="E6" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="97"/>
-      <c r="G6" s="98" t="s">
+      <c r="F6" s="72"/>
+      <c r="G6" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="91" t="s">
+      <c r="H6" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="A7" s="94">
+      <c r="A7" s="69">
         <v>2.4</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="97" t="s">
+      <c r="B7" s="64"/>
+      <c r="C7" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="90" t="s">
+      <c r="D7" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="98" t="s">
+      <c r="E7" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="97"/>
-      <c r="G7" s="98" t="s">
+      <c r="F7" s="72"/>
+      <c r="G7" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="91" t="s">
+      <c r="H7" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="57" t="s">
+      <c r="I7" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="A8" s="94">
+      <c r="A8" s="69">
         <v>2.5</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="97" t="s">
+      <c r="B8" s="64"/>
+      <c r="C8" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="90" t="s">
+      <c r="D8" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="98" t="s">
+      <c r="E8" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="98" t="s">
+      <c r="F8" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="97"/>
-      <c r="H8" s="92" t="s">
+      <c r="G8" s="72"/>
+      <c r="H8" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.2">
-      <c r="A9" s="95">
+      <c r="A9" s="70">
         <v>2.6</v>
       </c>
-      <c r="B9" s="96"/>
-      <c r="C9" s="97" t="s">
+      <c r="B9" s="71"/>
+      <c r="C9" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="97"/>
-      <c r="G9" s="100" t="s">
+      <c r="F9" s="72"/>
+      <c r="G9" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="93" t="s">
+      <c r="H9" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="57" t="s">
+      <c r="I9" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="120" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="57">
+      <c r="B10" s="56">
         <v>1</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="D10" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="I10" s="57" t="s">
+      <c r="I10" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="120" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="57">
+      <c r="B11" s="56">
         <v>1</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="56" t="s">
+      <c r="G11" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="57" t="s">
+      <c r="I11" s="56" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.2">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="B12" s="57">
+      <c r="B12" s="56">
         <v>1</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G12" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="H12" s="56" t="s">
+      <c r="H12" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="57" t="s">
+      <c r="I12" s="56" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3434,90 +3738,90 @@
     <mergeCell ref="A14:C16"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H3 H5:H9 H13:H1048576">
-    <cfRule type="containsText" dxfId="41" priority="22" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="71" priority="22" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="23" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="70" priority="23" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="24" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="69" priority="24" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="containsText" dxfId="38" priority="19" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="68" priority="19" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="20" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="67" priority="20" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="21" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="66" priority="21" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="65" priority="16" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="64" priority="17" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="63" priority="18" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="62" priority="13" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="61" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="60" priority="15" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="59" priority="10" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="58" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="12" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="57" priority="12" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="8" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="55" priority="8" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="9" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="54" priority="9" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="53" priority="4" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="52" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="51" priority="6" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:I12">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="48" priority="3" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I10)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3528,10 +3832,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3549,66 +3853,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="33" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-    </row>
-    <row r="3" spans="1:10" s="52" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" s="51" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="34" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3622,19 +3926,19 @@
       <c r="D4" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="57" t="s">
+      <c r="I4" s="56" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3648,129 +3952,152 @@
       <c r="D5" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="64" t="s">
+      <c r="G5" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="56" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:10" s="76" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A6" s="76">
         <v>3.3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="56" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="120" x14ac:dyDescent="0.2">
-      <c r="A7" s="57">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3.3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.2">
+      <c r="A8" s="56">
         <v>3.4</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B8" s="56">
         <v>1</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C8" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D8" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E8" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F8" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="56" t="s">
+      <c r="G8" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H8" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="57" t="s">
+      <c r="I8" s="56" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.2">
-      <c r="A8" s="57">
+    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.2">
+      <c r="A9" s="56">
         <v>3.5</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B9" s="56">
         <v>1</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C9" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D9" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E9" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F9" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G9" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="56" t="s">
+      <c r="H9" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I9" s="56" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.2">
-      <c r="A9" s="57">
+    <row r="10" spans="1:10" ht="120" x14ac:dyDescent="0.2">
+      <c r="A10" s="56">
         <v>3.6</v>
       </c>
-      <c r="B9" s="57">
+      <c r="B10" s="56">
         <v>1</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C10" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D10" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E10" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F10" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G10" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H10" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="I9" s="57" t="s">
+      <c r="I10" s="56" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3778,47 +4105,69 @@
   <mergeCells count="1">
     <mergeCell ref="A2:D2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H3 H10:H1048576 H5:H6 I7:I9">
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Invalid Test">
+  <conditionalFormatting sqref="H1:H3 H11:H1048576 H5 I8:I10 H7">
+    <cfRule type="containsText" dxfId="47" priority="25" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="46" priority="26" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="45" priority="27" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="41" priority="19" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="40" priority="20" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="39" priority="21" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="containsText" dxfId="38" priority="16" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",I7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="18" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",H6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",H6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Invalid Test">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Invalid Test">
       <formula>NOT(ISERROR(SEARCH("Invalid Test",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3828,6 +4177,274 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" style="76" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="76" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="76" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" style="76" customWidth="1"/>
+    <col min="5" max="5" width="55.5" style="76" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="76" customWidth="1"/>
+    <col min="7" max="7" width="30.5" style="76" customWidth="1"/>
+    <col min="8" max="8" width="17" style="76" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" style="76" customWidth="1"/>
+    <col min="10" max="10" width="31" style="76" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="76"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="50"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" s="51" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="76">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="I4" s="56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="76">
+        <v>4.2</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="63" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="76">
+        <v>4.3</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="56"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="56"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="56"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="56"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H1:H3 H10:H1048576 H5 I7:I9">
+    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",I4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",I5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="12" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",H6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",H6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",H6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Invalid Test">
+      <formula>NOT(ISERROR(SEARCH("Invalid Test",I6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
@@ -3843,333 +4460,333 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
     </row>
     <row r="3" spans="1:13" ht="41" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41" t="s">
+      <c r="A3" s="36"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="40"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="40"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="39"/>
     </row>
     <row r="5" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="43" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="40"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="39"/>
     </row>
     <row r="6" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="40"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="39"/>
     </row>
     <row r="7" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="44" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="38">
         <v>18</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="46" t="s">
+      <c r="F7" s="44"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="38">
         <v>0</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="38">
         <v>0</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="38">
         <v>18</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="46">
         <f>I7/E7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="40"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="44" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="38">
         <v>8</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="46" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="38">
         <v>0</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="38">
         <v>0</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="38">
         <v>8</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="46">
         <f>I8/E8</f>
         <v>0</v>
       </c>
-      <c r="M8" s="40"/>
+      <c r="M8" s="39"/>
     </row>
     <row r="9" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="44" t="s">
+      <c r="A9" s="36"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="38">
         <v>19</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="46" t="s">
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="38">
         <v>0</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="38">
         <v>0</v>
       </c>
-      <c r="K9" s="39">
+      <c r="K9" s="38">
         <v>19</v>
       </c>
-      <c r="L9" s="47">
+      <c r="L9" s="46">
         <f t="shared" ref="L9:L11" si="0">I9/E9</f>
         <v>0</v>
       </c>
-      <c r="M9" s="40"/>
+      <c r="M9" s="39"/>
     </row>
     <row r="10" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="44" t="s">
+      <c r="A10" s="36"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="38">
         <v>20</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="46" t="s">
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="38">
         <v>0</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="38">
         <v>0</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10" s="38">
         <v>20</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M10" s="40"/>
+      <c r="M10" s="39"/>
     </row>
     <row r="11" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="44" t="s">
+      <c r="A11" s="36"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="38">
         <v>42</v>
       </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="46" t="s">
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="38">
         <v>0</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="38">
         <v>0</v>
       </c>
-      <c r="K11" s="39">
+      <c r="K11" s="38">
         <v>42</v>
       </c>
-      <c r="L11" s="47">
+      <c r="L11" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" s="40"/>
+      <c r="M11" s="39"/>
     </row>
     <row r="12" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="40"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="39"/>
     </row>
     <row r="13" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="49">
+      <c r="D13" s="39"/>
+      <c r="E13" s="48">
         <f>SUM(E7:E12)</f>
         <v>107</v>
       </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49">
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48">
         <v>0</v>
       </c>
-      <c r="K13" s="49">
+      <c r="K13" s="48">
         <v>0</v>
       </c>
-      <c r="L13" s="47">
+      <c r="L13" s="46">
         <f>I13/E13</f>
         <v>0</v>
       </c>
-      <c r="M13" s="40"/>
+      <c r="M13" s="39"/>
     </row>
     <row r="14" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>